<commit_message>
we can write in one cell
</commit_message>
<xml_diff>
--- a/apache-poi/src/main/resources/prime-factors-scenarios.xlsx
+++ b/apache-poi/src/main/resources/prime-factors-scenarios.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ericmignot\IdeaProjects\sandbox\apache-poi\src\test\java\sandbox\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ericmignot\IdeaProjects\sandbox\apache-poi\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -408,13 +408,13 @@
   <dimension ref="B2:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22.42578125" style="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Travis now aware of what to do
</commit_message>
<xml_diff>
--- a/apache-poi/src/main/resources/prime-factors-scenarios.xlsx
+++ b/apache-poi/src/main/resources/prime-factors-scenarios.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ericmignot\IdeaProjects\sandbox\apache-poi\src\main\resources\"/>
     </mc:Choice>
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>can decompose 2</t>
   </si>
@@ -60,12 +60,16 @@
   </si>
   <si>
     <t>5, 5, 5</t>
+  </si>
+  <si>
+    <t>seen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -413,8 +417,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="22.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
@@ -443,6 +447,9 @@
       <c r="D5" s="1">
         <v>2</v>
       </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">

</xml_diff>